<commit_message>
dashboard per jenis alat berat dan kapasitas final
</commit_message>
<xml_diff>
--- a/Benchmark_Per_Alat_Berat_Data_Baru.xlsx
+++ b/Benchmark_Per_Alat_Berat_Data_Baru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEBE44-C669-4B2A-A9A9-DAD393A851B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE74B86E-24EB-414B-8301-146B72AB8CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rapor_Unit_Aktif" sheetId="1" r:id="rId1"/>
@@ -1188,7 +1188,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6422,7 +6422,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K149" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K149" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K149">
+      <sortCondition ref="A1:A149"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6431,9 +6435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6834,11 +6838,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6867,7 +6872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -6884,7 +6889,7 @@
         <v>4507</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -6901,7 +6906,7 @@
         <v>4248</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -6918,7 +6923,7 @@
         <v>3908</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -6935,7 +6940,7 @@
         <v>4463</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>172</v>
       </c>
@@ -6952,7 +6957,7 @@
         <v>4489</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -6969,7 +6974,7 @@
         <v>4948</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>4420</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>172</v>
       </c>
@@ -7003,7 +7008,7 @@
         <v>4792</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -7020,7 +7025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -7037,7 +7042,7 @@
         <v>1072.3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -7054,7 +7059,7 @@
         <v>3665</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>172</v>
       </c>
@@ -7071,7 +7076,7 @@
         <v>2613</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -7088,7 +7093,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -7105,7 +7110,7 @@
         <v>3923</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>172</v>
       </c>
@@ -7139,7 +7144,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -7156,7 +7161,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -7173,7 +7178,7 @@
         <v>3901</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -7190,7 +7195,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -7224,7 +7229,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>172</v>
       </c>
@@ -7241,7 +7246,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -7258,7 +7263,7 @@
         <v>4344</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -7292,7 +7297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -7309,7 +7314,7 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -7326,7 +7331,7 @@
         <v>3485</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -7343,7 +7348,7 @@
         <v>4822</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>172</v>
       </c>
@@ -7360,7 +7365,7 @@
         <v>4364</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>172</v>
       </c>
@@ -7377,7 +7382,7 @@
         <v>4840</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>172</v>
       </c>
@@ -7394,7 +7399,7 @@
         <v>3383</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -7411,7 +7416,7 @@
         <v>5566</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -7428,7 +7433,7 @@
         <v>4536</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>172</v>
       </c>
@@ -7445,7 +7450,7 @@
         <v>4154</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -7462,7 +7467,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>172</v>
       </c>
@@ -7479,7 +7484,7 @@
         <v>4949</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -7513,7 +7518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -7547,7 +7552,7 @@
         <v>545.1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -7564,7 +7569,7 @@
         <v>135.1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -7581,7 +7586,7 @@
         <v>848.29999999999973</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -7598,7 +7603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -7615,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -7633,7 +7638,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E46" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A1:E46" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TRONTON"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>